<commit_message>
update smaller excel files
</commit_message>
<xml_diff>
--- a/data/smaller.xlsx
+++ b/data/smaller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianyandell/Documents/Research/ewing/ewing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A3807C-AEB7-0044-B6C4-6E8975AD8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67C6AAB7-D50F-0F4B-8CED-669F8EAE03B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52220" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
+    <workbookView xWindow="52220" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
   </bookViews>
   <sheets>
     <sheet name="organism.features" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956A585-82A1-4C49-A77C-0D68492FFCAA}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1427,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9189E1F-80A5-2E4B-ACD1-CDB87453E092}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1.5.5: enable user-named species; fix various logic issues
</commit_message>
<xml_diff>
--- a/data/smaller.xlsx
+++ b/data/smaller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianyandell/Documents/Research/ewing/ewing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67C6AAB7-D50F-0F4B-8CED-669F8EAE03B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADACF8E3-1073-7847-9CE1-988E2772608B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52220" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
+    <workbookView xWindow="52420" yWindow="-120" windowWidth="15260" windowHeight="17440" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
   </bookViews>
   <sheets>
     <sheet name="organism.features" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,10 +714,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>

</xml_diff>